<commit_message>
random forests, new glms
</commit_message>
<xml_diff>
--- a/other regions/other studies.xlsx
+++ b/other regions/other studies.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="641">
   <si>
     <t>FP richness</t>
   </si>
@@ -1818,9 +1818,6 @@
     <t># water bodies w/o FP</t>
   </si>
   <si>
-    <t>e-mailed for data 7/21/2014</t>
-  </si>
-  <si>
     <t>Rank Percentile</t>
   </si>
   <si>
@@ -1974,9 +1971,6 @@
     <t>Great Britain - 2004</t>
   </si>
   <si>
-    <t>e-mailed for data 7/21/2014 - re-emailed 8/6/2014</t>
-  </si>
-  <si>
     <t>e-mailed (Duigan) for data 7/22/2014 - response 7/24 - replied 7/26 - Duigan out until 9/7</t>
   </si>
   <si>
@@ -1989,7 +1983,16 @@
     <t>~509</t>
   </si>
   <si>
-    <t>e-mailed for most recent version - 8/14/2014</t>
+    <t>e-mailed for data 7/21/2014 - replied 7/22 - re-emailed 8/6/2014</t>
+  </si>
+  <si>
+    <t>e-mailed for most recent version - 8/14/2014 - received same day</t>
+  </si>
+  <si>
+    <t>Communication notes</t>
+  </si>
+  <si>
+    <t>e-mailed for Pall data 7/21/2014 - re-e-mail Trei &amp; Pall 8/15/2014</t>
   </si>
 </sst>
 </file>
@@ -2000,7 +2003,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2048,6 +2051,14 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2080,7 +2091,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2092,6 +2103,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2179,11 +2191,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61599232"/>
-        <c:axId val="47569088"/>
+        <c:axId val="69080576"/>
+        <c:axId val="67280896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61599232"/>
+        <c:axId val="69080576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2212,7 +2224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47569088"/>
+        <c:crossAx val="67280896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2220,7 +2232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47569088"/>
+        <c:axId val="67280896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2249,7 +2261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61599232"/>
+        <c:crossAx val="69080576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2374,11 +2386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="56949248"/>
-        <c:axId val="64495616"/>
+        <c:axId val="66800128"/>
+        <c:axId val="67282624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56949248"/>
+        <c:axId val="66800128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2407,7 +2419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64495616"/>
+        <c:crossAx val="67282624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2415,7 +2427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64495616"/>
+        <c:axId val="67282624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2456,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56949248"/>
+        <c:crossAx val="66800128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -4790,8 +4802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4837,7 +4849,7 @@
         <v>553</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -5743,10 +5755,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B28" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C28">
         <v>89000</v>
@@ -5777,10 +5789,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C29">
         <v>89000</v>
@@ -5811,10 +5823,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B30" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C30">
         <v>89000</v>
@@ -5845,10 +5857,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B31" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C31">
         <v>89000</v>
@@ -5879,10 +5891,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B32" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C32">
         <v>89000</v>
@@ -5913,16 +5925,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C33">
         <v>89000</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E33">
         <v>1124</v>
@@ -5947,10 +5959,10 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B34" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C34">
         <v>89000</v>
@@ -5981,10 +5993,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B35" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C35">
         <v>89000</v>
@@ -6014,10 +6026,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B36" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C36">
         <v>89000</v>
@@ -6048,10 +6060,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B37" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C37">
         <v>89000</v>
@@ -6082,10 +6094,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B38" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C38">
         <v>89000</v>
@@ -6116,10 +6128,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B39" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C39">
         <v>89000</v>
@@ -6150,10 +6162,10 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B40" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C40">
         <v>89000</v>
@@ -6184,16 +6196,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B41" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C41">
         <v>89000</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E41">
         <v>3447</v>
@@ -6218,10 +6230,10 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B42" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C42">
         <v>89000</v>
@@ -6252,10 +6264,10 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B43" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C43">
         <v>89000</v>
@@ -6341,7 +6353,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6378,6 +6390,9 @@
       <c r="G1" s="8" t="s">
         <v>580</v>
       </c>
+      <c r="H1" s="11" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6474,7 +6489,7 @@
         <v>146</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -6500,7 +6515,7 @@
         <v>146</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -6526,7 +6541,7 @@
         <v>146</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>582</v>
+        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -6580,16 +6595,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>634</v>
+      </c>
+      <c r="B10" t="s">
+        <v>635</v>
+      </c>
+      <c r="D10" t="s">
         <v>636</v>
       </c>
-      <c r="B10" t="s">
-        <v>637</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="H10" s="3" t="s">
         <v>638</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -7918,16 +7933,16 @@
         <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>588</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>500</v>
@@ -7935,7 +7950,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B2">
         <v>537</v>
@@ -8071,7 +8086,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -8156,7 +8171,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B15">
         <v>175</v>
@@ -8207,7 +8222,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B18">
         <v>90</v>
@@ -8363,7 +8378,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B27">
         <v>83</v>
@@ -8482,7 +8497,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B34">
         <v>89</v>
@@ -8635,7 +8650,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B43">
         <v>19</v>
@@ -8723,7 +8738,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B48">
         <v>25</v>
@@ -8757,7 +8772,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B50">
         <v>31</v>
@@ -8774,7 +8789,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B51">
         <v>42</v>
@@ -8791,7 +8806,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B52">
         <v>28</v>
@@ -8859,7 +8874,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -8944,7 +8959,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -8978,7 +8993,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B63">
         <v>5</v>
@@ -9046,7 +9061,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B67">
         <v>14</v>
@@ -9063,7 +9078,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -9097,7 +9112,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -9202,7 +9217,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B76">
         <v>10</v>
@@ -9307,7 +9322,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -9324,7 +9339,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -9378,7 +9393,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -9395,7 +9410,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -9429,7 +9444,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -9446,7 +9461,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -9463,7 +9478,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -9480,7 +9495,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B92">
         <v>4</v>
@@ -9514,7 +9529,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -9554,7 +9569,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -9571,7 +9586,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -9588,7 +9603,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -9625,7 +9640,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -9642,7 +9657,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -9659,7 +9674,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -9676,7 +9691,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B103">
         <v>21</v>
@@ -9693,7 +9708,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B104">
         <v>11</v>
@@ -9710,7 +9725,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B105">
         <v>8</v>
@@ -9727,7 +9742,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B106">
         <v>5</v>
@@ -9744,7 +9759,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B107">
         <v>2</v>
@@ -9761,7 +9776,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B108">
         <v>2</v>
@@ -9778,7 +9793,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -9795,7 +9810,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -9829,7 +9844,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -9846,7 +9861,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B113">
         <v>1</v>

</xml_diff>